<commit_message>
Project documentation has been updated.
</commit_message>
<xml_diff>
--- a/Docs/DB.xlsx
+++ b/Docs/DB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>offer</t>
   </si>
@@ -79,6 +79,45 @@
   </si>
   <si>
     <t>client_designation</t>
+  </si>
+  <si>
+    <t>Primary Key</t>
+  </si>
+  <si>
+    <t>Foreign Key</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>bank_id</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>bank_name</t>
+  </si>
+  <si>
+    <t>bsnk_logo</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>processing_fees</t>
+  </si>
+  <si>
+    <t>loan_amount</t>
+  </si>
+  <si>
+    <t>loan_tenure</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -412,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -578,12 +617,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>